<commit_message>
Manejo correcto de Simulacion
</commit_message>
<xml_diff>
--- a/Input/Constante.xlsx
+++ b/Input/Constante.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/moises/Desktop/Produccion-Tesis/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B73D533-5F59-0B41-99A4-72597BB1EC7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB948AA1-9D1C-994D-A8EB-BF9E83782726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15640" firstSheet="5" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="940" windowWidth="24500" windowHeight="15200" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Costo Corte" sheetId="5" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1029" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1030" uniqueCount="168">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -30862,8 +30862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:L1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -30906,510 +30906,541 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="3">
-        <v>0</v>
-      </c>
-      <c r="C2" s="3">
-        <v>0</v>
-      </c>
-      <c r="D2" s="3">
-        <v>0</v>
-      </c>
-      <c r="E2" s="3">
-        <v>0</v>
-      </c>
-      <c r="F2" s="3">
-        <v>0</v>
-      </c>
-      <c r="G2" s="3">
-        <v>0</v>
-      </c>
-      <c r="H2" s="3">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>142.80387717065091</v>
-      </c>
-      <c r="J2" s="3">
-        <v>0</v>
-      </c>
-      <c r="K2" s="3">
-        <v>0</v>
-      </c>
-      <c r="L2" s="3"/>
+      <c r="B2" s="4">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4">
+        <v>94</v>
+      </c>
+      <c r="D2" s="4">
+        <v>335</v>
+      </c>
+      <c r="E2" s="4">
+        <v>1011</v>
+      </c>
+      <c r="F2" s="4">
+        <v>2804</v>
+      </c>
+      <c r="G2" s="4">
+        <v>3343</v>
+      </c>
+      <c r="H2" s="4">
+        <v>3690</v>
+      </c>
+      <c r="I2" s="4">
+        <v>5036</v>
+      </c>
+      <c r="J2" s="61">
+        <v>0</v>
+      </c>
+      <c r="K2" s="61">
+        <v>0</v>
+      </c>
+      <c r="L2" s="61">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B3" s="3">
-        <v>0</v>
-      </c>
-      <c r="C3" s="3">
-        <v>0</v>
-      </c>
-      <c r="D3" s="3">
-        <v>0</v>
-      </c>
-      <c r="E3" s="3">
-        <v>0</v>
-      </c>
-      <c r="F3" s="3">
-        <v>0</v>
-      </c>
-      <c r="G3" s="3">
-        <v>0</v>
-      </c>
-      <c r="H3" s="3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>160.3552694634545</v>
-      </c>
-      <c r="J3" s="3">
-        <v>0</v>
-      </c>
-      <c r="K3" s="3">
-        <v>0</v>
-      </c>
-      <c r="L3" s="3"/>
+      <c r="B3" s="4">
+        <v>10</v>
+      </c>
+      <c r="C3" s="4">
+        <v>62</v>
+      </c>
+      <c r="D3" s="4">
+        <v>354</v>
+      </c>
+      <c r="E3" s="4">
+        <v>156</v>
+      </c>
+      <c r="F3" s="4">
+        <v>1713</v>
+      </c>
+      <c r="G3" s="4">
+        <v>1603</v>
+      </c>
+      <c r="H3" s="4">
+        <v>1890</v>
+      </c>
+      <c r="I3" s="4">
+        <v>1854</v>
+      </c>
+      <c r="J3" s="61">
+        <v>0</v>
+      </c>
+      <c r="K3" s="61">
+        <v>0</v>
+      </c>
+      <c r="L3" s="61">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B4" s="3">
-        <v>0</v>
-      </c>
-      <c r="C4" s="3">
-        <v>0</v>
-      </c>
-      <c r="D4" s="3">
-        <v>0</v>
-      </c>
-      <c r="E4" s="3">
-        <v>0</v>
-      </c>
-      <c r="F4" s="3">
-        <v>0</v>
-      </c>
-      <c r="G4" s="3">
-        <v>0</v>
-      </c>
-      <c r="H4" s="3">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>77.996375391144909</v>
-      </c>
-      <c r="J4" s="3">
-        <v>0</v>
-      </c>
-      <c r="K4" s="3">
-        <v>0</v>
-      </c>
-      <c r="L4" s="3"/>
+      <c r="B4" s="4">
+        <v>3</v>
+      </c>
+      <c r="C4" s="4">
+        <v>57</v>
+      </c>
+      <c r="D4" s="4">
+        <v>64</v>
+      </c>
+      <c r="E4" s="4">
+        <v>556</v>
+      </c>
+      <c r="F4" s="4">
+        <v>76</v>
+      </c>
+      <c r="G4" s="4">
+        <v>818</v>
+      </c>
+      <c r="H4" s="4">
+        <v>1382</v>
+      </c>
+      <c r="I4" s="4">
+        <v>1449</v>
+      </c>
+      <c r="J4" s="61">
+        <v>0</v>
+      </c>
+      <c r="K4" s="61">
+        <v>0</v>
+      </c>
+      <c r="L4" s="61">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B5" s="3">
-        <v>0</v>
-      </c>
-      <c r="C5" s="3">
-        <v>0</v>
-      </c>
-      <c r="D5" s="3">
-        <v>0</v>
-      </c>
-      <c r="E5" s="3">
-        <v>0</v>
-      </c>
-      <c r="F5" s="3">
-        <v>0</v>
-      </c>
-      <c r="G5" s="3">
-        <v>0</v>
-      </c>
-      <c r="H5" s="3">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5" s="3">
-        <v>0</v>
-      </c>
-      <c r="K5" s="3">
-        <v>0</v>
-      </c>
-      <c r="L5" s="3"/>
+      <c r="B5" s="4">
+        <v>5</v>
+      </c>
+      <c r="C5" s="4">
+        <v>3</v>
+      </c>
+      <c r="D5" s="4">
+        <v>17</v>
+      </c>
+      <c r="E5" s="4">
+        <v>45</v>
+      </c>
+      <c r="F5" s="4">
+        <v>123</v>
+      </c>
+      <c r="G5" s="4">
+        <v>382</v>
+      </c>
+      <c r="H5" s="4">
+        <v>54</v>
+      </c>
+      <c r="I5" s="4">
+        <v>513</v>
+      </c>
+      <c r="J5" s="61">
+        <v>0</v>
+      </c>
+      <c r="K5" s="61">
+        <v>0</v>
+      </c>
+      <c r="L5" s="61">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B6" s="3">
-        <v>0</v>
-      </c>
-      <c r="C6" s="3">
-        <v>0</v>
-      </c>
-      <c r="D6" s="3">
-        <v>0</v>
-      </c>
-      <c r="E6" s="3">
-        <v>0</v>
-      </c>
-      <c r="F6" s="3">
-        <v>0</v>
-      </c>
-      <c r="G6" s="3">
-        <v>0</v>
-      </c>
-      <c r="H6" s="3">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>330.0755918623459</v>
-      </c>
-      <c r="J6" s="3">
-        <v>0</v>
-      </c>
-      <c r="K6" s="3">
-        <v>0</v>
-      </c>
-      <c r="L6" s="3"/>
+      <c r="B6" s="4">
+        <v>26</v>
+      </c>
+      <c r="C6" s="4">
+        <v>87</v>
+      </c>
+      <c r="D6" s="4">
+        <v>348</v>
+      </c>
+      <c r="E6" s="4">
+        <v>477</v>
+      </c>
+      <c r="F6" s="4">
+        <v>735</v>
+      </c>
+      <c r="G6" s="4">
+        <v>457</v>
+      </c>
+      <c r="H6" s="4">
+        <v>1911</v>
+      </c>
+      <c r="I6" s="4">
+        <v>2835</v>
+      </c>
+      <c r="J6" s="61">
+        <v>0</v>
+      </c>
+      <c r="K6" s="61">
+        <v>0</v>
+      </c>
+      <c r="L6" s="61">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B7" s="3">
-        <v>0</v>
-      </c>
-      <c r="C7" s="3">
-        <v>0</v>
-      </c>
-      <c r="D7" s="3">
-        <v>0</v>
-      </c>
-      <c r="E7" s="3">
-        <v>0</v>
-      </c>
-      <c r="F7" s="3">
-        <v>0</v>
-      </c>
-      <c r="G7" s="3">
-        <v>0</v>
-      </c>
-      <c r="H7" s="3">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>723.97513666034843</v>
-      </c>
-      <c r="J7" s="3">
-        <v>0</v>
-      </c>
-      <c r="K7" s="3">
-        <v>0</v>
-      </c>
-      <c r="L7" s="3"/>
+      <c r="B7" s="4">
+        <v>26</v>
+      </c>
+      <c r="C7" s="4">
+        <v>41</v>
+      </c>
+      <c r="D7" s="4">
+        <v>431</v>
+      </c>
+      <c r="E7" s="4">
+        <v>237</v>
+      </c>
+      <c r="F7" s="4">
+        <v>847</v>
+      </c>
+      <c r="G7" s="4">
+        <v>1221</v>
+      </c>
+      <c r="H7" s="4">
+        <v>1274</v>
+      </c>
+      <c r="I7" s="4">
+        <v>1806</v>
+      </c>
+      <c r="J7" s="61">
+        <v>0</v>
+      </c>
+      <c r="K7" s="61">
+        <v>0</v>
+      </c>
+      <c r="L7" s="61">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B8" s="3">
-        <v>0</v>
-      </c>
-      <c r="C8" s="3">
-        <v>0</v>
-      </c>
-      <c r="D8" s="3">
-        <v>0</v>
-      </c>
-      <c r="E8" s="3">
-        <v>0</v>
-      </c>
-      <c r="F8" s="3">
-        <v>0</v>
-      </c>
-      <c r="G8" s="3">
-        <v>0</v>
-      </c>
-      <c r="H8" s="3">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>666.82700030564888</v>
-      </c>
-      <c r="J8" s="3">
-        <v>0</v>
-      </c>
-      <c r="K8" s="3">
-        <v>0</v>
-      </c>
-      <c r="L8" s="3"/>
+      <c r="B8" s="4">
+        <v>37</v>
+      </c>
+      <c r="C8" s="4">
+        <v>84</v>
+      </c>
+      <c r="D8" s="4">
+        <v>141</v>
+      </c>
+      <c r="E8" s="4">
+        <v>1.2909999999999999</v>
+      </c>
+      <c r="F8" s="4">
+        <v>926</v>
+      </c>
+      <c r="G8" s="4">
+        <v>1243</v>
+      </c>
+      <c r="H8" s="4">
+        <v>2532</v>
+      </c>
+      <c r="I8" s="4">
+        <v>2655</v>
+      </c>
+      <c r="J8" s="61">
+        <v>0</v>
+      </c>
+      <c r="K8" s="61">
+        <v>0</v>
+      </c>
+      <c r="L8" s="61">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B9" s="3">
-        <v>0</v>
-      </c>
-      <c r="C9" s="3">
-        <v>0</v>
-      </c>
-      <c r="D9" s="3">
-        <v>0</v>
-      </c>
-      <c r="E9" s="3">
-        <v>0</v>
-      </c>
-      <c r="F9" s="3">
-        <v>0</v>
-      </c>
-      <c r="G9" s="3">
-        <v>0</v>
-      </c>
-      <c r="H9" s="3">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>293.18804112919048</v>
-      </c>
-      <c r="J9" s="3">
-        <v>0</v>
-      </c>
-      <c r="K9" s="3">
-        <v>0</v>
-      </c>
-      <c r="L9" s="3"/>
+      <c r="B9" s="4">
+        <v>5</v>
+      </c>
+      <c r="C9" s="4">
+        <v>27</v>
+      </c>
+      <c r="D9" s="4">
+        <v>129</v>
+      </c>
+      <c r="E9" s="4">
+        <v>511</v>
+      </c>
+      <c r="F9" s="4">
+        <v>599</v>
+      </c>
+      <c r="G9" s="4">
+        <v>20</v>
+      </c>
+      <c r="H9" s="4">
+        <v>1610</v>
+      </c>
+      <c r="I9" s="4">
+        <v>701</v>
+      </c>
+      <c r="J9" s="61">
+        <v>0</v>
+      </c>
+      <c r="K9" s="61">
+        <v>0</v>
+      </c>
+      <c r="L9" s="61">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B10" s="3">
-        <v>0</v>
-      </c>
-      <c r="C10" s="3">
-        <v>0</v>
-      </c>
-      <c r="D10" s="3">
-        <v>0</v>
-      </c>
-      <c r="E10" s="3">
-        <v>0</v>
-      </c>
-      <c r="F10" s="3">
-        <v>0</v>
-      </c>
-      <c r="G10" s="3">
-        <v>0</v>
-      </c>
-      <c r="H10" s="3">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10" s="3">
-        <v>0</v>
-      </c>
-      <c r="K10" s="3">
-        <v>0</v>
-      </c>
-      <c r="L10" s="3"/>
+      <c r="B10" s="4">
+        <v>1</v>
+      </c>
+      <c r="C10" s="4">
+        <v>11</v>
+      </c>
+      <c r="D10" s="4">
+        <v>269</v>
+      </c>
+      <c r="E10" s="4">
+        <v>3</v>
+      </c>
+      <c r="F10" s="4">
+        <v>797</v>
+      </c>
+      <c r="G10" s="4">
+        <v>1344</v>
+      </c>
+      <c r="H10" s="4">
+        <v>929</v>
+      </c>
+      <c r="I10" s="4">
+        <v>777</v>
+      </c>
+      <c r="J10" s="61">
+        <v>0</v>
+      </c>
+      <c r="K10" s="61">
+        <v>0</v>
+      </c>
+      <c r="L10" s="61">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B11" s="3">
-        <v>0</v>
-      </c>
-      <c r="C11" s="3">
-        <v>0</v>
-      </c>
-      <c r="D11" s="3">
-        <v>0</v>
-      </c>
-      <c r="E11" s="3">
-        <v>0</v>
-      </c>
-      <c r="F11" s="3">
-        <v>0</v>
-      </c>
-      <c r="G11" s="3">
-        <v>0</v>
-      </c>
-      <c r="H11" s="3">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11" s="3">
-        <v>0</v>
-      </c>
-      <c r="K11" s="3">
-        <v>0</v>
-      </c>
-      <c r="L11" s="3"/>
+      <c r="B11" s="4">
+        <v>2</v>
+      </c>
+      <c r="C11" s="4">
+        <v>2</v>
+      </c>
+      <c r="D11" s="4">
+        <v>84</v>
+      </c>
+      <c r="E11" s="4">
+        <v>44</v>
+      </c>
+      <c r="F11" s="4">
+        <v>179</v>
+      </c>
+      <c r="G11" s="4">
+        <v>103</v>
+      </c>
+      <c r="H11" s="4">
+        <v>381</v>
+      </c>
+      <c r="I11" s="4">
+        <v>404</v>
+      </c>
+      <c r="J11" s="61">
+        <v>0</v>
+      </c>
+      <c r="K11" s="61">
+        <v>0</v>
+      </c>
+      <c r="L11" s="61">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B12" s="3">
-        <v>0</v>
-      </c>
-      <c r="C12" s="3">
-        <v>0</v>
-      </c>
-      <c r="D12" s="3">
-        <v>0</v>
-      </c>
-      <c r="E12" s="3">
-        <v>0</v>
-      </c>
-      <c r="F12" s="3">
-        <v>0</v>
-      </c>
-      <c r="G12" s="3">
-        <v>0</v>
-      </c>
-      <c r="H12" s="3">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-      <c r="J12" s="3">
-        <v>0</v>
-      </c>
-      <c r="K12" s="3">
-        <v>0</v>
-      </c>
-      <c r="L12" s="3"/>
+      <c r="B12" s="4">
+        <v>6</v>
+      </c>
+      <c r="C12" s="4">
+        <v>16</v>
+      </c>
+      <c r="D12" s="4">
+        <v>81</v>
+      </c>
+      <c r="E12" s="4">
+        <v>264</v>
+      </c>
+      <c r="F12" s="4">
+        <v>262</v>
+      </c>
+      <c r="G12" s="4">
+        <v>3</v>
+      </c>
+      <c r="H12" s="4">
+        <v>266</v>
+      </c>
+      <c r="I12" s="4">
+        <v>176</v>
+      </c>
+      <c r="J12" s="61">
+        <v>0</v>
+      </c>
+      <c r="K12" s="61">
+        <v>0</v>
+      </c>
+      <c r="L12" s="61">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B13" s="3">
-        <v>0</v>
-      </c>
-      <c r="C13" s="3">
-        <v>0</v>
-      </c>
-      <c r="D13" s="3">
-        <v>0</v>
-      </c>
-      <c r="E13" s="3">
-        <v>0</v>
-      </c>
-      <c r="F13" s="3">
-        <v>0</v>
-      </c>
-      <c r="G13" s="3">
-        <v>0</v>
-      </c>
-      <c r="H13" s="3">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-      <c r="J13" s="3">
-        <v>0</v>
-      </c>
-      <c r="K13" s="3">
-        <v>0</v>
-      </c>
-      <c r="L13" s="3"/>
+      <c r="B13" s="4">
+        <v>3</v>
+      </c>
+      <c r="C13" s="4">
+        <v>1</v>
+      </c>
+      <c r="D13" s="4">
+        <v>39</v>
+      </c>
+      <c r="E13" s="4">
+        <v>118</v>
+      </c>
+      <c r="F13" s="4">
+        <v>120</v>
+      </c>
+      <c r="G13" s="4">
+        <v>157</v>
+      </c>
+      <c r="H13" s="4">
+        <v>51</v>
+      </c>
+      <c r="I13" s="4">
+        <v>106</v>
+      </c>
+      <c r="J13" s="61">
+        <v>0</v>
+      </c>
+      <c r="K13" s="61">
+        <v>0</v>
+      </c>
+      <c r="L13" s="61">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B14" s="3">
-        <v>0</v>
-      </c>
-      <c r="C14" s="3">
-        <v>0</v>
-      </c>
-      <c r="D14" s="3">
-        <v>0</v>
-      </c>
-      <c r="E14" s="3">
-        <v>0</v>
-      </c>
-      <c r="F14" s="3">
-        <v>0</v>
-      </c>
-      <c r="G14" s="3">
-        <v>0</v>
-      </c>
-      <c r="H14" s="3">
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <v>52.360462189477182</v>
-      </c>
-      <c r="J14" s="3">
-        <v>0</v>
-      </c>
-      <c r="K14" s="3">
-        <v>0</v>
-      </c>
-      <c r="L14" s="3"/>
+      <c r="B14" s="4">
+        <v>9</v>
+      </c>
+      <c r="C14" s="4">
+        <v>23</v>
+      </c>
+      <c r="D14" s="4">
+        <v>95</v>
+      </c>
+      <c r="E14" s="4">
+        <v>276</v>
+      </c>
+      <c r="F14" s="4">
+        <v>50</v>
+      </c>
+      <c r="G14" s="4">
+        <v>152</v>
+      </c>
+      <c r="H14" s="4">
+        <v>749</v>
+      </c>
+      <c r="I14" s="4">
+        <v>167</v>
+      </c>
+      <c r="J14" s="61">
+        <v>0</v>
+      </c>
+      <c r="K14" s="61">
+        <v>0</v>
+      </c>
+      <c r="L14" s="61">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B15" s="3">
-        <v>0</v>
-      </c>
-      <c r="C15" s="3">
-        <v>0</v>
-      </c>
-      <c r="D15" s="3">
-        <v>0</v>
-      </c>
-      <c r="E15" s="3">
-        <v>0</v>
-      </c>
-      <c r="F15" s="3">
-        <v>0</v>
-      </c>
-      <c r="G15" s="3">
-        <v>0</v>
-      </c>
-      <c r="H15" s="3">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-      <c r="J15" s="3">
-        <v>0</v>
-      </c>
-      <c r="K15" s="3">
-        <v>0</v>
-      </c>
-      <c r="L15" s="3"/>
+      <c r="B15" s="4">
+        <v>8</v>
+      </c>
+      <c r="C15" s="4">
+        <v>31</v>
+      </c>
+      <c r="D15" s="4">
+        <v>120</v>
+      </c>
+      <c r="E15" s="4">
+        <v>468</v>
+      </c>
+      <c r="F15" s="4">
+        <v>366</v>
+      </c>
+      <c r="G15" s="4">
+        <v>240</v>
+      </c>
+      <c r="H15" s="4">
+        <v>684</v>
+      </c>
+      <c r="I15" s="4">
+        <v>890</v>
+      </c>
+      <c r="J15" s="61">
+        <v>0</v>
+      </c>
+      <c r="K15" s="61">
+        <v>0</v>
+      </c>
+      <c r="L15" s="61">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -38820,7 +38851,7 @@
   <dimension ref="A1:P1000"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:L15"/>
+      <selection activeCell="B2" sqref="B2:I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -52247,9 +52278,9 @@
   </sheetPr>
   <dimension ref="A1:AA45"/>
   <sheetViews>
-    <sheetView zoomScale="184" zoomScaleNormal="199" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="199" workbookViewId="0">
       <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M4" sqref="M4"/>
+      <selection pane="topRight" activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Modelo con Valor residual
</commit_message>
<xml_diff>
--- a/Input/Constante.xlsx
+++ b/Input/Constante.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/moises/Desktop/Produccion-Tesis/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F862F752-5CC6-D042-9079-B978EFBB4248}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1354485B-E4FE-014F-8373-289C04C65C43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="940" windowWidth="24500" windowHeight="15200" firstSheet="5" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="940" windowWidth="24500" windowHeight="15200" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Costo Corte" sheetId="5" r:id="rId1"/>
@@ -29313,8 +29313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:CM1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U14" sqref="U14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:CM2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -52278,9 +52278,9 @@
   </sheetPr>
   <dimension ref="A1:AA45"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="199" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="199" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>